<commit_message>
fixed a small error
</commit_message>
<xml_diff>
--- a/Study plan/Statistics.xlsx
+++ b/Study plan/Statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nextcloud\Documents\Pouya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Pouya\BD-And-Microservices\Study plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2E0CE-5863-452B-B501-BFFEDAE3619E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C508700-9383-4E3D-8A27-AEF2C1D40DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="3240" windowWidth="38340" windowHeight="10185" xr2:uid="{CCA7CEBC-7415-400C-A7BD-323C6ECD14A5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{CCA7CEBC-7415-400C-A7BD-323C6ECD14A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEA76C0-7C8D-4922-8340-6DA704D135C3}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +897,7 @@
         <v>40</v>
       </c>
       <c r="B48" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -905,7 +905,7 @@
         <v>41</v>
       </c>
       <c r="B49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>